<commit_message>
bug fixes funcionarios total
</commit_message>
<xml_diff>
--- a/storage/AGENDA.xlsx
+++ b/storage/AGENDA.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7740"/>
+    <workbookView windowWidth="13230" windowHeight="11955"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1045,10 +1045,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1063,6 +1063,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1081,15 +1096,22 @@
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1104,7 +1126,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1127,7 +1149,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1140,16 +1170,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1165,7 +1188,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1173,39 +1203,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1218,7 +1218,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1230,43 +1230,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1284,7 +1248,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1308,13 +1290,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1332,7 +1314,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1344,61 +1392,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1440,16 +1440,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1460,15 +1460,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1488,28 +1479,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1517,8 +1491,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1537,153 +1511,179 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2053,27 +2053,27 @@
   <sheetPr/>
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F$1:G$1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="47.375" customWidth="1"/>
-    <col min="3" max="3" width="14.75" customWidth="1"/>
-    <col min="4" max="4" width="14.75" style="1" customWidth="1"/>
-    <col min="5" max="5" width="9.375" customWidth="1"/>
-    <col min="6" max="6" width="9.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="47.3733333333333" customWidth="1"/>
+    <col min="3" max="3" width="14.7533333333333" customWidth="1"/>
+    <col min="4" max="4" width="14.7533333333333" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.37333333333333" customWidth="1"/>
+    <col min="6" max="6" width="9.87333333333333" style="1" customWidth="1"/>
     <col min="7" max="9" width="12" customWidth="1"/>
-    <col min="10" max="10" width="35.875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="22.375" customWidth="1"/>
-    <col min="12" max="13" width="12.375" customWidth="1"/>
-    <col min="14" max="14" width="18.875" customWidth="1"/>
-    <col min="15" max="15" width="18.875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="18.875" customWidth="1"/>
-    <col min="17" max="17" width="18.875" style="4" customWidth="1"/>
-    <col min="18" max="18" width="18.875" customWidth="1"/>
-    <col min="21" max="21" width="12.75" customWidth="1"/>
+    <col min="10" max="10" width="35.8733333333333" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.3733333333333" customWidth="1"/>
+    <col min="12" max="13" width="12.3733333333333" customWidth="1"/>
+    <col min="14" max="14" width="18.8733333333333" customWidth="1"/>
+    <col min="15" max="15" width="18.8733333333333" style="3" customWidth="1"/>
+    <col min="16" max="16" width="18.8733333333333" customWidth="1"/>
+    <col min="17" max="17" width="18.8733333333333" style="4" customWidth="1"/>
+    <col min="18" max="18" width="18.8733333333333" customWidth="1"/>
+    <col min="21" max="21" width="12.7533333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -2143,7 +2143,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="5">
-        <v>14172</v>
+        <v>22511</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>21</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="5">
-        <v>14173</v>
+        <v>22512</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>32</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="5">
-        <v>14174</v>
+        <v>22513</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="5">
-        <v>14175</v>
+        <v>22514</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>47</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="5">
-        <v>14176</v>
+        <v>22515</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>53</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="5">
-        <v>14177</v>
+        <v>22516</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>60</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="5">
-        <v>14178</v>
+        <v>22517</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>67</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="5">
-        <v>14179</v>
+        <v>22518</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>74</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="5">
-        <v>14180</v>
+        <v>22519</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>81</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="5">
-        <v>14181</v>
+        <v>22520</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>88</v>
@@ -2705,7 +2705,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="5">
-        <v>14182</v>
+        <v>22521</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>94</v>
@@ -2760,7 +2760,7 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="5">
-        <v>14183</v>
+        <v>22522</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>100</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="5">
-        <v>14184</v>
+        <v>22523</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>107</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="5">
-        <v>14185</v>
+        <v>22524</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>113</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5">
-        <v>14186</v>
+        <v>22525</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>119</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="5">
-        <v>14187</v>
+        <v>22526</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>126</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="5">
-        <v>14188</v>
+        <v>22527</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>132</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="5">
-        <v>14189</v>
+        <v>22528</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>138</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="5">
-        <v>14190</v>
+        <v>22529</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>144</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="5">
-        <v>14191</v>
+        <v>22530</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>150</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="5">
-        <v>14192</v>
+        <v>22531</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>157</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="5">
-        <v>14193</v>
+        <v>22532</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>164</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="5">
-        <v>14194</v>
+        <v>22533</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>171</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="5">
-        <v>14195</v>
+        <v>22534</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>177</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="5">
-        <v>14196</v>
+        <v>22535</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>183</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="5">
-        <v>14197</v>
+        <v>22536</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>189</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="5">
-        <v>14198</v>
+        <v>22537</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>196</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="5">
-        <v>14199</v>
+        <v>22538</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>203</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="5">
-        <v>14200</v>
+        <v>22539</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>210</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="5">
-        <v>14201</v>
+        <v>22540</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>217</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="5">
-        <v>14202</v>
+        <v>22541</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>224</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="5">
-        <v>14203</v>
+        <v>22542</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>231</v>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="5">
-        <v>14204</v>
+        <v>22543</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>238</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="5">
-        <v>14205</v>
+        <v>22544</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>244</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="5">
-        <v>14206</v>
+        <v>22545</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>251</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="5">
-        <v>14207</v>
+        <v>22546</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>258</v>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="5">
-        <v>14208</v>
+        <v>22547</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>265</v>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="5">
-        <v>14209</v>
+        <v>22548</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>270</v>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="5">
-        <v>14210</v>
+        <v>22549</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>277</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="5">
-        <v>14211</v>
+        <v>22550</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>284</v>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="5">
-        <v>14212</v>
+        <v>22551</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>291</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="5">
-        <v>14213</v>
+        <v>22552</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>297</v>
@@ -4499,7 +4499,7 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="5">
-        <v>14214</v>
+        <v>22553</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>303</v>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="5">
-        <v>14215</v>
+        <v>22554</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>310</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="5">
-        <v>14216</v>
+        <v>22555</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>316</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="5">
-        <v>14217</v>
+        <v>22556</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>322</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="5">
-        <v>14218</v>
+        <v>22557</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>328</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="5">
-        <v>14219</v>
+        <v>22558</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>334</v>

</xml_diff>

<commit_message>
Updated Autorizador y Seguimiento
</commit_message>
<xml_diff>
--- a/storage/AGENDA.xlsx
+++ b/storage/AGENDA.xlsx
@@ -1045,10 +1045,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy;@"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -1065,8 +1065,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1080,17 +1103,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1105,37 +1127,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1156,22 +1148,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1193,9 +1187,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1218,7 +1218,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1230,7 +1236,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1242,13 +1362,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1260,145 +1398,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1440,21 +1440,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1479,13 +1464,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1501,6 +1490,32 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1522,168 +1537,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2053,8 +2053,8 @@
   <sheetPr/>
   <dimension ref="A1:U49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B15" sqref="B$1:B$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="15.75"/>
@@ -2143,7 +2143,7 @@
     </row>
     <row r="2" spans="1:21">
       <c r="A2" s="5">
-        <v>22511</v>
+        <v>22514</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>21</v>
@@ -2200,7 +2200,7 @@
     </row>
     <row r="3" spans="1:21">
       <c r="A3" s="5">
-        <v>22512</v>
+        <v>22515</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>32</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="4" spans="1:21">
       <c r="A4" s="5">
-        <v>22513</v>
+        <v>22516</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>39</v>
@@ -2314,7 +2314,7 @@
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="5">
-        <v>22514</v>
+        <v>22517</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>47</v>
@@ -2369,7 +2369,7 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="5">
-        <v>22515</v>
+        <v>22518</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>53</v>
@@ -2424,7 +2424,7 @@
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="5">
-        <v>22516</v>
+        <v>22519</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>60</v>
@@ -2481,7 +2481,7 @@
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="5">
-        <v>22517</v>
+        <v>22520</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>67</v>
@@ -2538,7 +2538,7 @@
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="5">
-        <v>22518</v>
+        <v>22521</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>74</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="5">
-        <v>22519</v>
+        <v>22522</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>81</v>
@@ -2650,7 +2650,7 @@
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="5">
-        <v>22520</v>
+        <v>22523</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>88</v>
@@ -2705,7 +2705,7 @@
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="5">
-        <v>22521</v>
+        <v>22524</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>94</v>
@@ -2760,7 +2760,7 @@
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="5">
-        <v>22522</v>
+        <v>22525</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>100</v>
@@ -2817,7 +2817,7 @@
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="5">
-        <v>22523</v>
+        <v>22526</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>107</v>
@@ -2872,7 +2872,7 @@
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="5">
-        <v>22524</v>
+        <v>22527</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>113</v>
@@ -2927,7 +2927,7 @@
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="5">
-        <v>22525</v>
+        <v>22528</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>119</v>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="5">
-        <v>22526</v>
+        <v>22529</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>126</v>
@@ -3039,7 +3039,7 @@
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="5">
-        <v>22527</v>
+        <v>22530</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>132</v>
@@ -3094,7 +3094,7 @@
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="5">
-        <v>22528</v>
+        <v>22531</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>138</v>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="5">
-        <v>22529</v>
+        <v>22532</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>144</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="5">
-        <v>22530</v>
+        <v>22533</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>150</v>
@@ -3255,7 +3255,7 @@
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="5">
-        <v>22531</v>
+        <v>22534</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>157</v>
@@ -3312,7 +3312,7 @@
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="5">
-        <v>22532</v>
+        <v>22535</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>164</v>
@@ -3367,7 +3367,7 @@
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="5">
-        <v>22533</v>
+        <v>22536</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>171</v>
@@ -3422,7 +3422,7 @@
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="5">
-        <v>22534</v>
+        <v>22537</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>177</v>
@@ -3479,7 +3479,7 @@
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="5">
-        <v>22535</v>
+        <v>22538</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>183</v>
@@ -3536,7 +3536,7 @@
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="5">
-        <v>22536</v>
+        <v>22539</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>189</v>
@@ -3593,7 +3593,7 @@
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="5">
-        <v>22537</v>
+        <v>22540</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>196</v>
@@ -3650,7 +3650,7 @@
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="5">
-        <v>22538</v>
+        <v>22541</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>203</v>
@@ -3707,7 +3707,7 @@
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="5">
-        <v>22539</v>
+        <v>22542</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>210</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="5">
-        <v>22540</v>
+        <v>22543</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>217</v>
@@ -3821,7 +3821,7 @@
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="5">
-        <v>22541</v>
+        <v>22544</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>224</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="5">
-        <v>22542</v>
+        <v>22545</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>231</v>
@@ -3935,7 +3935,7 @@
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="5">
-        <v>22543</v>
+        <v>22546</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>238</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="5">
-        <v>22544</v>
+        <v>22547</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>244</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="5">
-        <v>22545</v>
+        <v>22548</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>251</v>
@@ -4102,7 +4102,7 @@
     </row>
     <row r="37" spans="1:21">
       <c r="A37" s="5">
-        <v>22546</v>
+        <v>22549</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>258</v>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="38" spans="1:21">
       <c r="A38" s="5">
-        <v>22547</v>
+        <v>22550</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>265</v>
@@ -4216,7 +4216,7 @@
     </row>
     <row r="39" spans="1:21">
       <c r="A39" s="5">
-        <v>22548</v>
+        <v>22551</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>270</v>
@@ -4273,7 +4273,7 @@
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="5">
-        <v>22549</v>
+        <v>22552</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>277</v>
@@ -4330,7 +4330,7 @@
     </row>
     <row r="41" spans="1:21">
       <c r="A41" s="5">
-        <v>22550</v>
+        <v>22553</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>284</v>
@@ -4387,7 +4387,7 @@
     </row>
     <row r="42" spans="1:21">
       <c r="A42" s="5">
-        <v>22551</v>
+        <v>22554</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>291</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="43" spans="1:21">
       <c r="A43" s="5">
-        <v>22552</v>
+        <v>22555</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>297</v>
@@ -4499,7 +4499,7 @@
     </row>
     <row r="44" spans="1:21">
       <c r="A44" s="5">
-        <v>22553</v>
+        <v>22556</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>303</v>
@@ -4556,7 +4556,7 @@
     </row>
     <row r="45" spans="1:21">
       <c r="A45" s="5">
-        <v>22554</v>
+        <v>22557</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>310</v>
@@ -4611,7 +4611,7 @@
     </row>
     <row r="46" spans="1:21">
       <c r="A46" s="5">
-        <v>22555</v>
+        <v>22558</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>316</v>
@@ -4666,7 +4666,7 @@
     </row>
     <row r="47" spans="1:21">
       <c r="A47" s="5">
-        <v>22556</v>
+        <v>22559</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>322</v>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="48" spans="1:21">
       <c r="A48" s="5">
-        <v>22557</v>
+        <v>22560</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>328</v>
@@ -4778,7 +4778,7 @@
     </row>
     <row r="49" spans="1:21">
       <c r="A49" s="5">
-        <v>22558</v>
+        <v>22561</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>334</v>

</xml_diff>